<commit_message>
feat: add algorithm to count Retention and Strength of memory for flashcard
</commit_message>
<xml_diff>
--- a/server/src/uploads/excels/235403/exam.3.mini-test3.xlsx
+++ b/server/src/uploads/excels/235403/exam.3.mini-test3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Project\toeic_prep\server\src\uploads\excels\235403\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3331E8-58F8-41BE-AE89-12E02BD9B2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177D9B4B-52A1-481C-BC35-1333F1EDBE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-163" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1885,7 +1885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1910,7 +1910,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2217,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L101"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2257,7 +2256,7 @@
       <c r="K1" s="15" t="s">
         <v>526</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="15" t="s">
         <v>527</v>
       </c>
     </row>
@@ -4701,6 +4700,9 @@
       </c>
       <c r="J75" s="11" t="s">
         <v>28</v>
+      </c>
+      <c r="K75">
+        <v>7</v>
       </c>
       <c r="L75" t="s">
         <v>539</v>

</xml_diff>